<commit_message>
Final Update: project is accomplished
</commit_message>
<xml_diff>
--- a/Europe_3_Factors.xlsx
+++ b/Europe_3_Factors.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
   <si>
     <t xml:space="preserve">Mkt-RF</t>
   </si>
@@ -32,6 +32,282 @@
   </si>
   <si>
     <t xml:space="preserve">RF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2012-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2013-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2014-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2015-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2016-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2019-08</t>
   </si>
 </sst>
 </file>
@@ -130,8 +406,8 @@
   </sheetPr>
   <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I41" activeCellId="0" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -159,8 +435,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>201201</v>
+      <c r="A2" s="0" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>5.69</v>
@@ -176,8 +452,8 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>201202</v>
+      <c r="A3" s="0" t="s">
+        <v>5</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>6.41</v>
@@ -193,8 +469,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>201203</v>
+      <c r="A4" s="0" t="s">
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.02</v>
@@ -210,8 +486,8 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>201204</v>
+      <c r="A5" s="0" t="s">
+        <v>7</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>-2.23</v>
@@ -227,8 +503,8 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
-        <v>201205</v>
+      <c r="A6" s="0" t="s">
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>-12.31</v>
@@ -244,8 +520,8 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
-        <v>201206</v>
+      <c r="A7" s="0" t="s">
+        <v>9</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>7.13</v>
@@ -261,8 +537,8 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>201207</v>
+      <c r="A8" s="0" t="s">
+        <v>10</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.56</v>
@@ -278,8 +554,8 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>201208</v>
+      <c r="A9" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>4.5</v>
@@ -295,8 +571,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>201209</v>
+      <c r="A10" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>3.49</v>
@@ -312,8 +588,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>201210</v>
+      <c r="A11" s="0" t="s">
+        <v>13</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>1.66</v>
@@ -329,8 +605,8 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>201211</v>
+      <c r="A12" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>2.27</v>
@@ -346,8 +622,8 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>201212</v>
+      <c r="A13" s="0" t="s">
+        <v>15</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>3.38</v>
@@ -363,8 +639,8 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>201301</v>
+      <c r="A14" s="0" t="s">
+        <v>16</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>6.2</v>
@@ -380,8 +656,8 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>201302</v>
+      <c r="A15" s="0" t="s">
+        <v>17</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>-2.49</v>
@@ -397,8 +673,8 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>201303</v>
+      <c r="A16" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>-0.54</v>
@@ -414,8 +690,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>201304</v>
+      <c r="A17" s="0" t="s">
+        <v>19</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>4.16</v>
@@ -431,8 +707,8 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>201305</v>
+      <c r="A18" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>1.06</v>
@@ -448,8 +724,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>201306</v>
+      <c r="A19" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>-4.64</v>
@@ -465,8 +741,8 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>201307</v>
+      <c r="A20" s="0" t="s">
+        <v>22</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>7.45</v>
@@ -482,8 +758,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>201308</v>
+      <c r="A21" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>-0.7</v>
@@ -499,8 +775,8 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>201309</v>
+      <c r="A22" s="0" t="s">
+        <v>24</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>7.04</v>
@@ -516,8 +792,8 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>201310</v>
+      <c r="A23" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>4.49</v>
@@ -533,8 +809,8 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
-        <v>201311</v>
+      <c r="A24" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>1.33</v>
@@ -550,8 +826,8 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>201312</v>
+      <c r="A25" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>2.37</v>
@@ -567,8 +843,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>201401</v>
+      <c r="A26" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>-3.03</v>
@@ -584,8 +860,8 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>201402</v>
+      <c r="A27" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>7.42</v>
@@ -601,8 +877,8 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
-        <v>201403</v>
+      <c r="A28" s="0" t="s">
+        <v>30</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>-0.55</v>
@@ -618,8 +894,8 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
-        <v>201404</v>
+      <c r="A29" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>1.77</v>
@@ -635,8 +911,8 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>201405</v>
+      <c r="A30" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>0.77</v>
@@ -652,8 +928,8 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>201406</v>
+      <c r="A31" s="0" t="s">
+        <v>33</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>-0.12</v>
@@ -669,8 +945,8 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <v>201407</v>
+      <c r="A32" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>-4.1</v>
@@ -686,8 +962,8 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
-        <v>201408</v>
+      <c r="A33" s="0" t="s">
+        <v>35</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>-0.02</v>
@@ -703,8 +979,8 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
-        <v>201409</v>
+      <c r="A34" s="0" t="s">
+        <v>36</v>
       </c>
       <c r="B34" s="0" t="n">
         <v>-3.79</v>
@@ -720,8 +996,8 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
-        <v>201410</v>
+      <c r="A35" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="B35" s="0" t="n">
         <v>-2.7</v>
@@ -737,8 +1013,8 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
-        <v>201411</v>
+      <c r="A36" s="0" t="s">
+        <v>38</v>
       </c>
       <c r="B36" s="0" t="n">
         <v>2.12</v>
@@ -754,8 +1030,8 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
-        <v>201412</v>
+      <c r="A37" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="B37" s="0" t="n">
         <v>-3.7</v>
@@ -771,8 +1047,8 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
-        <v>201501</v>
+      <c r="A38" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>-0.3</v>
@@ -788,8 +1064,8 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <v>201502</v>
+      <c r="A39" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>6.21</v>
@@ -805,8 +1081,8 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <v>201503</v>
+      <c r="A40" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>-2.28</v>
@@ -822,8 +1098,8 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>201504</v>
+      <c r="A41" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>4.79</v>
@@ -839,8 +1115,8 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>201505</v>
+      <c r="A42" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>-0.15</v>
@@ -856,8 +1132,8 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>201506</v>
+      <c r="A43" s="0" t="s">
+        <v>45</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>-2.84</v>
@@ -873,8 +1149,8 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
-        <v>201507</v>
+      <c r="A44" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>2.39</v>
@@ -890,8 +1166,8 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
-        <v>201508</v>
+      <c r="A45" s="0" t="s">
+        <v>47</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>-6.02</v>
@@ -907,8 +1183,8 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
-        <v>201509</v>
+      <c r="A46" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>-4.27</v>
@@ -924,8 +1200,8 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
-        <v>201510</v>
+      <c r="A47" s="0" t="s">
+        <v>49</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>6.19</v>
@@ -941,8 +1217,8 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
-        <v>201511</v>
+      <c r="A48" s="0" t="s">
+        <v>50</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>-1.49</v>
@@ -958,8 +1234,8 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
-        <v>201512</v>
+      <c r="A49" s="0" t="s">
+        <v>51</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>-1.86</v>
@@ -975,8 +1251,8 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
-        <v>201601</v>
+      <c r="A50" s="0" t="s">
+        <v>52</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>-6.43</v>
@@ -992,8 +1268,8 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
-        <v>201602</v>
+      <c r="A51" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>-1.71</v>
@@ -1009,8 +1285,8 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
-        <v>201603</v>
+      <c r="A52" s="0" t="s">
+        <v>54</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>6.7</v>
@@ -1026,8 +1302,8 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
-        <v>201604</v>
+      <c r="A53" s="0" t="s">
+        <v>55</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>2.38</v>
@@ -1043,8 +1319,8 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
-        <v>201605</v>
+      <c r="A54" s="0" t="s">
+        <v>56</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>-0.38</v>
@@ -1060,8 +1336,8 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
-        <v>201606</v>
+      <c r="A55" s="0" t="s">
+        <v>57</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>-5.01</v>
@@ -1077,8 +1353,8 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
-        <v>201607</v>
+      <c r="A56" s="0" t="s">
+        <v>58</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>4.44</v>
@@ -1094,8 +1370,8 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
-        <v>201608</v>
+      <c r="A57" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0.77</v>
@@ -1111,8 +1387,8 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
-        <v>201609</v>
+      <c r="A58" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>0.95</v>
@@ -1128,8 +1404,8 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
-        <v>201610</v>
+      <c r="A59" s="0" t="s">
+        <v>61</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>-3.08</v>
@@ -1145,8 +1421,8 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="n">
-        <v>201611</v>
+      <c r="A60" s="0" t="s">
+        <v>62</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>-2.5</v>
@@ -1162,8 +1438,8 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
-        <v>201612</v>
+      <c r="A61" s="0" t="s">
+        <v>63</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>4.72</v>
@@ -1179,8 +1455,8 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
-        <v>201701</v>
+      <c r="A62" s="0" t="s">
+        <v>64</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>2.84</v>
@@ -1196,8 +1472,8 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
-        <v>201702</v>
+      <c r="A63" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>0.68</v>
@@ -1213,8 +1489,8 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
-        <v>201703</v>
+      <c r="A64" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>4.27</v>
@@ -1230,8 +1506,8 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
-        <v>201704</v>
+      <c r="A65" s="0" t="s">
+        <v>67</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>4.63</v>
@@ -1247,8 +1523,8 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="n">
-        <v>201705</v>
+      <c r="A66" s="0" t="s">
+        <v>68</v>
       </c>
       <c r="B66" s="0" t="n">
         <v>5.03</v>
@@ -1264,8 +1540,8 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="n">
-        <v>201706</v>
+      <c r="A67" s="0" t="s">
+        <v>69</v>
       </c>
       <c r="B67" s="0" t="n">
         <v>-0.67</v>
@@ -1281,8 +1557,8 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="n">
-        <v>201707</v>
+      <c r="A68" s="0" t="s">
+        <v>70</v>
       </c>
       <c r="B68" s="0" t="n">
         <v>3.49</v>
@@ -1298,8 +1574,8 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="n">
-        <v>201708</v>
+      <c r="A69" s="0" t="s">
+        <v>71</v>
       </c>
       <c r="B69" s="0" t="n">
         <v>0.11</v>
@@ -1315,8 +1591,8 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="n">
-        <v>201709</v>
+      <c r="A70" s="0" t="s">
+        <v>72</v>
       </c>
       <c r="B70" s="0" t="n">
         <v>2.72</v>
@@ -1332,8 +1608,8 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="n">
-        <v>201710</v>
+      <c r="A71" s="0" t="s">
+        <v>73</v>
       </c>
       <c r="B71" s="0" t="n">
         <v>0.59</v>
@@ -1349,8 +1625,8 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="n">
-        <v>201711</v>
+      <c r="A72" s="0" t="s">
+        <v>74</v>
       </c>
       <c r="B72" s="0" t="n">
         <v>-0.01</v>
@@ -1366,8 +1642,8 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="n">
-        <v>201712</v>
+      <c r="A73" s="0" t="s">
+        <v>75</v>
       </c>
       <c r="B73" s="0" t="n">
         <v>1.47</v>
@@ -1383,8 +1659,8 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="n">
-        <v>201801</v>
+      <c r="A74" s="0" t="s">
+        <v>76</v>
       </c>
       <c r="B74" s="0" t="n">
         <v>5.52</v>
@@ -1400,8 +1676,8 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="n">
-        <v>201802</v>
+      <c r="A75" s="0" t="s">
+        <v>77</v>
       </c>
       <c r="B75" s="0" t="n">
         <v>-5.35</v>
@@ -1417,8 +1693,8 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="n">
-        <v>201803</v>
+      <c r="A76" s="0" t="s">
+        <v>78</v>
       </c>
       <c r="B76" s="0" t="n">
         <v>-0.71</v>
@@ -1434,8 +1710,8 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="n">
-        <v>201804</v>
+      <c r="A77" s="0" t="s">
+        <v>79</v>
       </c>
       <c r="B77" s="0" t="n">
         <v>2.2</v>
@@ -1451,8 +1727,8 @@
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="n">
-        <v>201805</v>
+      <c r="A78" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="B78" s="0" t="n">
         <v>-2.73</v>
@@ -1468,8 +1744,8 @@
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="n">
-        <v>201806</v>
+      <c r="A79" s="0" t="s">
+        <v>81</v>
       </c>
       <c r="B79" s="0" t="n">
         <v>-0.92</v>
@@ -1485,8 +1761,8 @@
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="n">
-        <v>201807</v>
+      <c r="A80" s="0" t="s">
+        <v>82</v>
       </c>
       <c r="B80" s="0" t="n">
         <v>2.69</v>
@@ -1502,8 +1778,8 @@
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="n">
-        <v>201808</v>
+      <c r="A81" s="0" t="s">
+        <v>83</v>
       </c>
       <c r="B81" s="0" t="n">
         <v>-2.65</v>
@@ -1519,8 +1795,8 @@
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="n">
-        <v>201809</v>
+      <c r="A82" s="0" t="s">
+        <v>84</v>
       </c>
       <c r="B82" s="0" t="n">
         <v>0.12</v>
@@ -1536,8 +1812,8 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="n">
-        <v>201810</v>
+      <c r="A83" s="0" t="s">
+        <v>85</v>
       </c>
       <c r="B83" s="0" t="n">
         <v>-8.54</v>
@@ -1553,8 +1829,8 @@
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="n">
-        <v>201811</v>
+      <c r="A84" s="0" t="s">
+        <v>86</v>
       </c>
       <c r="B84" s="0" t="n">
         <v>-1.31</v>
@@ -1570,8 +1846,8 @@
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="n">
-        <v>201812</v>
+      <c r="A85" s="0" t="s">
+        <v>87</v>
       </c>
       <c r="B85" s="0" t="n">
         <v>-4.59</v>
@@ -1587,8 +1863,8 @@
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="n">
-        <v>201901</v>
+      <c r="A86" s="0" t="s">
+        <v>88</v>
       </c>
       <c r="B86" s="0" t="n">
         <v>6.19</v>
@@ -1604,8 +1880,8 @@
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="n">
-        <v>201902</v>
+      <c r="A87" s="0" t="s">
+        <v>89</v>
       </c>
       <c r="B87" s="0" t="n">
         <v>2.93</v>
@@ -1621,8 +1897,8 @@
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="n">
-        <v>201903</v>
+      <c r="A88" s="0" t="s">
+        <v>90</v>
       </c>
       <c r="B88" s="0" t="n">
         <v>0.58</v>
@@ -1638,8 +1914,8 @@
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="n">
-        <v>201904</v>
+      <c r="A89" s="0" t="s">
+        <v>91</v>
       </c>
       <c r="B89" s="0" t="n">
         <v>3.7</v>
@@ -1655,8 +1931,8 @@
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="n">
-        <v>201905</v>
+      <c r="A90" s="0" t="s">
+        <v>92</v>
       </c>
       <c r="B90" s="0" t="n">
         <v>-5.34</v>
@@ -1672,8 +1948,8 @@
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="n">
-        <v>201906</v>
+      <c r="A91" s="0" t="s">
+        <v>93</v>
       </c>
       <c r="B91" s="0" t="n">
         <v>5.87</v>
@@ -1689,8 +1965,8 @@
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="n">
-        <v>201907</v>
+      <c r="A92" s="0" t="s">
+        <v>94</v>
       </c>
       <c r="B92" s="0" t="n">
         <v>-2.56</v>
@@ -1706,8 +1982,8 @@
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="n">
-        <v>201908</v>
+      <c r="A93" s="0" t="s">
+        <v>95</v>
       </c>
       <c r="B93" s="0" t="n">
         <v>-2.39</v>

</xml_diff>